<commit_message>
testing rust/python hybrid output
</commit_message>
<xml_diff>
--- a/Filenames.xlsx
+++ b/Filenames.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/120104837ef5190b/4. Programs/Git/Word Template Generator/Python-Word-Template-Generator/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/120104837ef5190b/4. Programs/Git/Word Template Generator/Python-Word-Template-Generator/Python-Word-Template-Generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="99" documentId="8_{11FA82D2-367D-4E07-8316-B2F76032CA20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D86B0CFD-A731-4337-B2BC-403A83E6B52D}"/>
+  <xr:revisionPtr revIDLastSave="101" documentId="8_{11FA82D2-367D-4E07-8316-B2F76032CA20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97D7EF67-E507-4AC1-A296-97544C0CB2F7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{BD469674-CA7A-49C4-9BCD-D31A6FA461CD}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="67">
   <si>
     <t>Title</t>
   </si>
@@ -301,10 +301,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -627,7 +623,7 @@
   <dimension ref="A1:Y11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,7 +710,7 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>48</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -814,6 +810,57 @@
       <c r="H3" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="I3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -840,6 +887,57 @@
       <c r="H4" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="I4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -866,6 +964,57 @@
       <c r="H5" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="I5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -892,6 +1041,57 @@
       <c r="H6" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="I6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -918,6 +1118,57 @@
       <c r="H7" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="I7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -944,6 +1195,57 @@
       <c r="H8" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="I8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -970,6 +1272,57 @@
       <c r="H9" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="I9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -996,6 +1349,57 @@
       <c r="H10" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="I10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="X10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y10" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -1021,6 +1425,57 @@
       </c>
       <c r="H11" s="1" t="s">
         <v>16</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="W11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="X11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y11" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>